<commit_message>
Fixed sample file for investor access
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_access.xlsx
+++ b/public/sample_uploads/investor_access.xlsx
@@ -20,7 +20,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t xml:space="preserve">First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Name</t>
+  </si>
   <si>
     <t xml:space="preserve">Email</t>
   </si>
@@ -28,10 +34,22 @@
     <t xml:space="preserve">Approved</t>
   </si>
   <si>
+    <t xml:space="preserve">Emp1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hero</t>
+  </si>
+  <si>
     <t xml:space="preserve">emp1@mycompany.com</t>
   </si>
   <si>
     <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emp2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Villain</t>
   </si>
   <si>
     <t xml:space="preserve">emp2@mycompany.com</t>
@@ -52,6 +70,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -159,101 +178,119 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="24.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="emp1@mycompany.com"/>
-    <hyperlink ref="A3" r:id="rId2" display="emp2@mycompany.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="emp1@mycompany.com"/>
+    <hyperlink ref="C3" r:id="rId2" display="emp2@mycompany.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Now added distribution payments based on commitment %
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_access.xlsx
+++ b/public/sample_uploads/investor_access.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Approved</t>
   </si>
   <si>
+    <t xml:space="preserve">Investor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emp1</t>
   </si>
   <si>
@@ -46,6 +49,9 @@
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
+    <t xml:space="preserve">Kalaari Capital</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emp2</t>
   </si>
   <si>
@@ -56,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accel</t>
   </si>
 </sst>
 </file>
@@ -181,10 +190,10 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="24.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.67"/>
@@ -207,7 +216,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -215,18 +226,20 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -234,18 +247,20 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>

</xml_diff>

<commit_message>
Moved import_upload file to shrine
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_access.xlsx
+++ b/public/sample_uploads/investor_access.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -34,9 +34,6 @@
     <t xml:space="preserve">Approved</t>
   </si>
   <si>
-    <t xml:space="preserve">Investor</t>
-  </si>
-  <si>
     <t xml:space="preserve">Emp1</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Kalaari Capital</t>
-  </si>
-  <si>
     <t xml:space="preserve">Emp2</t>
   </si>
   <si>
@@ -62,9 +56,6 @@
   </si>
   <si>
     <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accel</t>
   </si>
 </sst>
 </file>
@@ -190,10 +181,10 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E:E"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="24.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.67"/>
@@ -216,9 +207,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -226,20 +215,18 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -247,20 +234,18 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>

</xml_diff>

<commit_message>
Investor access has ability to supress emails
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_access.xlsx
+++ b/public/sample_uploads/investor_access.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -34,28 +34,31 @@
     <t xml:space="preserve">Approved</t>
   </si>
   <si>
+    <t xml:space="preserve">Send Confirmation Email</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emp1</t>
   </si>
   <si>
     <t xml:space="preserve">Hero</t>
   </si>
   <si>
-    <t xml:space="preserve">emp1@mycompany.com</t>
+    <t xml:space="preserve">emp10@mycompany.com</t>
   </si>
   <si>
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emp2</t>
   </si>
   <si>
     <t xml:space="preserve">Villain</t>
   </si>
   <si>
-    <t xml:space="preserve">emp2@mycompany.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
+    <t xml:space="preserve">emp20@mycompany.com</t>
   </si>
 </sst>
 </file>
@@ -181,10 +184,10 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E:E"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="24.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.67"/>
@@ -207,7 +210,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -215,18 +220,20 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -234,18 +241,20 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -289,8 +298,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="emp1@mycompany.com"/>
-    <hyperlink ref="C3" r:id="rId2" display="emp2@mycompany.com"/>
+    <hyperlink ref="C3" r:id="rId1" display="emp20@mycompany.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Misc fixes 1 (#70)
* Added button to trigger vested job

* Added carry for fund unit settings

* Added AllocationRun model

* Added kyc document generation

* Added document generation for KYC

* Fixed fund ratios date

* Added document generation for KYC

* Fixed tests
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_access.xlsx
+++ b/public/sample_uploads/investor_access.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028A54A6-0D76-4DED-9D26-6F68B5F77C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972F04D3-F1B4-45ED-91B3-C31019BFEDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>First Name</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Send Confirmation Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>WhatsApp Enabled</t>
   </si>
 </sst>
 </file>
@@ -437,23 +443,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.53125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="24.1328125" customWidth="1"/>
-    <col min="5" max="5" width="50.6640625" customWidth="1"/>
-    <col min="6" max="7" width="19.33203125" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.265625" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" customWidth="1"/>
+    <col min="2" max="6" width="24.1328125" customWidth="1"/>
+    <col min="7" max="7" width="50.6640625" customWidth="1"/>
+    <col min="8" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="13.265625" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -467,17 +473,23 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -490,18 +502,24 @@
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2">
+        <v>9999999999</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -514,18 +532,24 @@
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2">
+        <v>8888888888</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -533,8 +557,10 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -542,8 +568,10 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -551,8 +579,10 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -560,6 +590,8 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Made import_upload_id not nil for interests
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_access.xlsx
+++ b/public/sample_uploads/investor_access.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E334012E-77E8-448E-932A-FE7CF37E3CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB501DFB-09B5-4135-9F09-56C1B82B59FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="735" windowWidth="23985" windowHeight="14265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Investments" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{83BA3124-B6FE-4205-BDF2-81792A950DC5}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{83BA3124-B6FE-4205-BDF2-81792A950DC5}">
       <text>
         <r>
           <rPr>
@@ -160,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{E6883A4C-AD0B-4E28-B15A-68E95CC5035E}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{E6883A4C-AD0B-4E28-B15A-68E95CC5035E}">
       <text>
         <r>
           <rPr>
@@ -185,7 +185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{24AA27D7-3E9A-49AD-A257-4178374BB37C}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{24AA27D7-3E9A-49AD-A257-4178374BB37C}">
       <text>
         <r>
           <rPr>
@@ -209,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{E84ECF22-555F-45CC-801C-CAA9565A7A68}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{E84ECF22-555F-45CC-801C-CAA9565A7A68}">
       <text>
         <r>
           <rPr>
@@ -233,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{D2029974-5B8A-4983-8D62-86AF426E1EBD}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{D2029974-5B8A-4983-8D62-86AF426E1EBD}">
       <text>
         <r>
           <rPr>
@@ -257,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{BA531C45-8A37-4F00-8B9F-AAFC95FB66F7}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{BA531C45-8A37-4F00-8B9F-AAFC95FB66F7}">
       <text>
         <r>
           <rPr>
@@ -286,7 +286,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>First Name</t>
   </si>
@@ -361,6 +361,9 @@
   </si>
   <si>
     <t>emp1@investor2.com</t>
+  </si>
+  <si>
+    <t>Email Enabled</t>
   </si>
 </sst>
 </file>
@@ -778,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E3" sqref="E3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.53125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -790,16 +793,17 @@
     <col min="2" max="2" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.06640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.06640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.53125" style="1"/>
+    <col min="5" max="5" width="21.86328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="35.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.06640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.53125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -813,25 +817,28 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -844,26 +851,29 @@
       <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>9999999999</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -876,26 +886,29 @@
       <c r="D3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>8888888888</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -908,35 +921,38 @@
       <c r="D4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>9999999999</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:J1048576" xr:uid="{3FF7EA7B-A53F-4EA8-A721-5DFDEF688BBB}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:K1048576" xr:uid="{3FF7EA7B-A53F-4EA8-A721-5DFDEF688BBB}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{96C495B5-CD28-456C-B71C-30C3D640770E}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{8AF39A48-7608-49C3-A2C2-C1635C260D5A}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{532CA2AB-D767-497B-92C0-C1E0762579E6}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{96C495B5-CD28-456C-B71C-30C3D640770E}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{8AF39A48-7608-49C3-A2C2-C1635C260D5A}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{532CA2AB-D767-497B-92C0-C1E0762579E6}"/>
     <hyperlink ref="D2" r:id="rId4" xr:uid="{12EAF395-45CB-40B4-A1CE-D25772FD434C}"/>
     <hyperlink ref="D3" r:id="rId5" xr:uid="{340D8B25-04DF-46B2-AB2C-710D95394AF7}"/>
     <hyperlink ref="D4" r:id="rId6" xr:uid="{7CAAA395-2C34-403F-B224-DD3D76E27A5E}"/>

</xml_diff>

<commit_message>
Custom notification attachments (#424)
* Made holdings optional in offer

* Added import of offers without holdings tests

* Bug fix for offer spa gen

* Added better support for attaching documents for custom notifications

* Added signed_document_already_exists? check for doc generation

* Removed support email as mandatory

* Passed ctx to save_rows for imports

* Fixed tests

* Fixed tests
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_access.xlsx
+++ b/public/sample_uploads/investor_access.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB501DFB-09B5-4135-9F09-56C1B82B59FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A70797-F521-46D9-9673-7BBE7A7716BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="735" windowWidth="23985" windowHeight="14265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -286,7 +286,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
   <si>
     <t>First Name</t>
   </si>
@@ -364,6 +364,54 @@
   </si>
   <si>
     <t>Email Enabled</t>
+  </si>
+  <si>
+    <t>Investor 3</t>
+  </si>
+  <si>
+    <t>Investor 4</t>
+  </si>
+  <si>
+    <t>Investor 5</t>
+  </si>
+  <si>
+    <t>Investor 6</t>
+  </si>
+  <si>
+    <t>Emp3</t>
+  </si>
+  <si>
+    <t>Emp4</t>
+  </si>
+  <si>
+    <t>Emp5</t>
+  </si>
+  <si>
+    <t>Emp6</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>emp1@investor3.com</t>
+  </si>
+  <si>
+    <t>emp1@investor4.com</t>
+  </si>
+  <si>
+    <t>emp1@investor5.com</t>
+  </si>
+  <si>
+    <t>emp1@investor6.com</t>
   </si>
 </sst>
 </file>
@@ -781,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E4"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.53125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -943,8 +991,124 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1111111111</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2222222222</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3333333333</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:K1048576" xr:uid="{3FF7EA7B-A53F-4EA8-A721-5DFDEF688BBB}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
@@ -956,9 +1120,13 @@
     <hyperlink ref="D2" r:id="rId4" xr:uid="{12EAF395-45CB-40B4-A1CE-D25772FD434C}"/>
     <hyperlink ref="D3" r:id="rId5" xr:uid="{340D8B25-04DF-46B2-AB2C-710D95394AF7}"/>
     <hyperlink ref="D4" r:id="rId6" xr:uid="{7CAAA395-2C34-403F-B224-DD3D76E27A5E}"/>
+    <hyperlink ref="D5" r:id="rId7" xr:uid="{14D1EF17-8CDB-4869-86E3-5130C0405FAD}"/>
+    <hyperlink ref="D6" r:id="rId8" xr:uid="{BB68ACFE-38C8-418A-8128-D674B3114D4B}"/>
+    <hyperlink ref="D7" r:id="rId9" xr:uid="{4A838F46-74F4-486D-97E8-E6D81BB7CD82}"/>
+    <hyperlink ref="D8" r:id="rId10" xr:uid="{55C4EED1-2A47-4CB4-8516-4507AAA1C324}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId7"/>
+  <legacyDrawing r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added better support for new advisor notification
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_access.xlsx
+++ b/public/sample_uploads/investor_access.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A70797-F521-46D9-9673-7BBE7A7716BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC1C299-EFF4-42BB-A4CA-5BFDBF0D8828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="735" windowWidth="23985" windowHeight="14265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -286,7 +286,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
   <si>
     <t>First Name</t>
   </si>
@@ -832,7 +832,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.53125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1105,6 +1105,18 @@
       </c>
       <c r="G8" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1234567789</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>